<commit_message>
adding serial killer vs zodiac charts
</commit_message>
<xml_diff>
--- a/killers_excel.xlsx
+++ b/killers_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b954984cd282067a/Desktop/Class_folder/Class Project/Horrorscopes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{1493A3A1-D195-4CCE-BE0F-B93F78F6773C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B71AFE9D-F432-4CF2-82F9-BAE512B3778B}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{1493A3A1-D195-4CCE-BE0F-B93F78F6773C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31E7106C-A1AE-4DA7-8522-EB051A859C0E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2569468D-C13A-4330-8DF5-F3EF403746FB}"/>
   </bookViews>
@@ -1663,7 +1663,7 @@
     <t>Last, First</t>
   </si>
   <si>
-    <t>DOB</t>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -2019,10 +2019,13 @@
   <dimension ref="A1:E500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -2371,7 +2374,7 @@
       <c r="B21" t="s">
         <v>31</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D21">
@@ -2609,7 +2612,7 @@
       <c r="B35" t="s">
         <v>47</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D35">
@@ -3323,7 +3326,7 @@
       <c r="B77" t="s">
         <v>91</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D77">
@@ -3629,7 +3632,7 @@
       <c r="B95" t="s">
         <v>110</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="1" t="s">
         <v>111</v>
       </c>
       <c r="D95">
@@ -3646,7 +3649,7 @@
       <c r="B96" t="s">
         <v>112</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D96">
@@ -3935,7 +3938,7 @@
       <c r="B113" t="s">
         <v>130</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="1" t="s">
         <v>131</v>
       </c>
       <c r="D113">
@@ -4751,7 +4754,7 @@
       <c r="B161" t="s">
         <v>179</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C161" s="1" t="s">
         <v>180</v>
       </c>
       <c r="D161">
@@ -5720,7 +5723,7 @@
       <c r="B218" t="s">
         <v>237</v>
       </c>
-      <c r="C218" t="s">
+      <c r="C218" s="1" t="s">
         <v>238</v>
       </c>
       <c r="D218">
@@ -5788,7 +5791,7 @@
       <c r="B222" t="s">
         <v>242</v>
       </c>
-      <c r="C222" t="s">
+      <c r="C222" s="1" t="s">
         <v>243</v>
       </c>
       <c r="D222">
@@ -5890,7 +5893,7 @@
       <c r="B228" t="s">
         <v>249</v>
       </c>
-      <c r="C228" t="s">
+      <c r="C228" s="1" t="s">
         <v>250</v>
       </c>
       <c r="D228">
@@ -6009,7 +6012,7 @@
       <c r="B235" t="s">
         <v>257</v>
       </c>
-      <c r="C235" t="s">
+      <c r="C235" s="1" t="s">
         <v>258</v>
       </c>
       <c r="D235">
@@ -7063,7 +7066,7 @@
       <c r="B297" t="s">
         <v>320</v>
       </c>
-      <c r="C297" t="s">
+      <c r="C297" s="1" t="s">
         <v>321</v>
       </c>
       <c r="D297" t="s">
@@ -7454,7 +7457,7 @@
       <c r="B320" t="s">
         <v>345</v>
       </c>
-      <c r="C320" t="s">
+      <c r="C320" s="1" t="s">
         <v>346</v>
       </c>
       <c r="D320">
@@ -7743,7 +7746,7 @@
       <c r="B337" t="s">
         <v>363</v>
       </c>
-      <c r="C337" t="s">
+      <c r="C337" s="1" t="s">
         <v>364</v>
       </c>
       <c r="D337">
@@ -8083,7 +8086,7 @@
       <c r="B357" t="s">
         <v>384</v>
       </c>
-      <c r="C357" t="s">
+      <c r="C357" s="1" t="s">
         <v>385</v>
       </c>
       <c r="D357">
@@ -8134,7 +8137,7 @@
       <c r="B360" t="s">
         <v>388</v>
       </c>
-      <c r="C360" t="s">
+      <c r="C360" s="1" t="s">
         <v>389</v>
       </c>
       <c r="D360">
@@ -8202,7 +8205,7 @@
       <c r="B364" t="s">
         <v>393</v>
       </c>
-      <c r="C364" t="s">
+      <c r="C364" s="1" t="s">
         <v>394</v>
       </c>
       <c r="D364">
@@ -8219,7 +8222,7 @@
       <c r="B365" t="s">
         <v>395</v>
       </c>
-      <c r="C365" t="s">
+      <c r="C365" s="1" t="s">
         <v>396</v>
       </c>
       <c r="D365">
@@ -8644,7 +8647,7 @@
       <c r="B390" t="s">
         <v>421</v>
       </c>
-      <c r="C390" t="s">
+      <c r="C390" s="1" t="s">
         <v>422</v>
       </c>
       <c r="D390">
@@ -9052,7 +9055,7 @@
       <c r="B414" t="s">
         <v>446</v>
       </c>
-      <c r="C414" t="s">
+      <c r="C414" s="1" t="s">
         <v>447</v>
       </c>
       <c r="D414">
@@ -9426,7 +9429,7 @@
       <c r="B436" t="s">
         <v>469</v>
       </c>
-      <c r="C436" t="s">
+      <c r="C436" s="1" t="s">
         <v>470</v>
       </c>
       <c r="D436">
@@ -9443,7 +9446,7 @@
       <c r="B437" t="s">
         <v>471</v>
       </c>
-      <c r="C437" t="s">
+      <c r="C437" s="1" t="s">
         <v>472</v>
       </c>
       <c r="D437">
@@ -9613,7 +9616,7 @@
       <c r="B447" t="s">
         <v>482</v>
       </c>
-      <c r="C447" t="s">
+      <c r="C447" s="1" t="s">
         <v>483</v>
       </c>
       <c r="D447">
@@ -10191,7 +10194,7 @@
       <c r="B481" t="s">
         <v>517</v>
       </c>
-      <c r="C481" t="s">
+      <c r="C481" s="1" t="s">
         <v>518</v>
       </c>
       <c r="D481">
@@ -10344,7 +10347,7 @@
       <c r="B490" t="s">
         <v>527</v>
       </c>
-      <c r="C490" t="s">
+      <c r="C490" s="1" t="s">
         <v>528</v>
       </c>
       <c r="D490">

</xml_diff>